<commit_message>
Update md and RS file for MS-ASAIRS
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASAIRS/MS-ASAIRS_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASAIRS/MS-ASAIRS_RequirementSpecification.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE01FC8-01E4-47A5-B3E5-B4EA716F1F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="570"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -20,8 +21,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmp4016" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmp4016" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-wenfa\AppData\Local\Temp\tmp4016.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -7034,7 +7035,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -7320,6 +7321,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7343,21 +7359,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -16835,34 +16836,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I950" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I950"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I950" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I950" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -16871,12 +16872,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A12:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16958,6 +16959,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -16993,6 +17011,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -17168,11 +17203,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L952"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:I15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -17221,132 +17258,132 @@
         <v>789</v>
       </c>
       <c r="F3" s="12">
-        <v>43634</v>
+        <v>44516</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -17359,12 +17396,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -17377,12 +17414,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -17395,12 +17432,12 @@
       <c r="C14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="30">
@@ -17413,60 +17450,60 @@
       <c r="C15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -40948,11 +40985,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -40960,6 +40992,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A907:B924 D907:I924 D86:I86 D87:H89 A95:E95 B102:B105 A179:B179 B321:I322 A574:I574 B600:I601 A595:B597 B92:G93 B96:E101 A439:I439 A544:I544 A675:I679 A727:I730 B379:D380 B386:D387 A408:I414 B420:I423 A640:I652 A658:I662 A687:I692 A698:I703 A709:I714 A756:I759 A778:I783 A789:I799 A809:I811 A817:I820 A826:I828 B177:B178 A299:B300 B520:I521 B576:F586 A653:B656 A663:B666 A682:B685 A693:B696 A704:B707 A715:B718 A731:B734 A751:B754 A773:B776 A784:B787 A812:B815 A821:B824 A829:B832 A834:I838 C203:I203 C341:I342 A359:I359 C360:I363 C440:I442 C545:I550 A623:I634 C614:C615 A765:I772 D839:I842 A844:I906 A575:F575 G575:I586 F424:F428 H424:H428 B94:E94 F94:G101 F574:F586 F299:F303 H299:H303 F282:F286 H282:H286 F323:F326 H323:H326 F369:I373 H374:H378 F379:I380 F386:I387 F499:G501 F502:I503 D602:H608 D613:E615 F613:G617 D609:G612 A189:I202 A339:I340 A760:B763 A800:B803 A839:B842 A938:I950 A925:D926 F925:I926 A20:I38 A64:I66 A68 C68:D68 A69:D70 I68:I70 F69:F70 A71:I71 A74:A75 C74:I75 A84:I84 A86:B89 I86:I89 B91:H91 H92:H105 F102:F105 A144:I161 B162:B166 A139:B143 B170:B174 B180:B181 D177:H179 D180 F180:H180 D181:H181 G175:I175 B175:E175 B167:I169 B182:I183 C204:H205 A213:I218 A219:B223 A224:I242 A243:B249 B211:I212 A250:I262 A263:B267 A268:I281 A282:B286 A287:I298 B301:B303 B304:I305 B306:B310 B311:I315 B316:B320 B323:B326 B354:B358 B369:D373 B374:B378 A393:I402 A403:B407 A456:I462 A463:B467 A468:I471 A472:B476 A477:I480 A481:B485 A486:I488 D494:H496 B499:D503 A510:I514 B515:B519 A522:I525 B556:I557 B558:B562 B563:I573 B598:B599 B616:E617 A618:B622 H609:H622 F618:F622 A635:B638 A668:I669 A671:B673 B670 A681:I681 B680:I680 A720:I721 A722:B725 A736:I737 A738:B741 A743:I750 A805:B805 A816 A825 A833 A843 A107:I138 B203:B210 A91:A105 A162:A175 I91:I175 A203:A212 A301:A338 B328:B338 A341:B353 B360:B368 F374:F378 B381:B385 B388:B392 A360:A392 B415:B419 A415:A423 A424:B438 A440:B455 B489:C498 A489:A509 B500:B509 A515:A538 A526:B543 B545:B555 B587:B591 B184:B188 F184:G184 A177:A188 I177:I225 B592:I594 B602:B615 A545:A617 I229:I638 I640:I805 I807 A807:B807 I809:I924">
@@ -47371,23 +47408,23 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F950">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F950" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E950">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E950" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G950">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G950" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H938:H950 H20:H924">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H938:H950 H20:H924" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H925:H937">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H925:H937" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"Message Deserialization, Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -47413,6 +47450,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -47461,15 +47507,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{869B59C6-9FF4-49E7-A701-55AF5B3B0EF5}">
   <ds:schemaRefs>
@@ -47486,6 +47523,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -47498,12 +47543,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>